<commit_message>
Add more works between 30 GHz and 40 GHz
</commit_message>
<xml_diff>
--- a/mmWave_osc_db.xlsx
+++ b/mmWave_osc_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamag\Nextcloud\Documents\TIMA\Doutorado\SOA\mmW_VCO_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5018988-1D69-4C2B-9A49-A1BC563AF92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2607480-BB76-483B-B4EF-24B7B08D44DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,6 +101,9 @@
     <author>tc={006B002D-006C-48CA-963D-002500E10057}</author>
     <author>tc={E80CD336-E602-49C5-8915-0A7EE86690F9}</author>
     <author>tc={535D1BA5-778F-4DA6-8BEA-A2E1949A80B1}</author>
+    <author>tc={2C8311BA-9217-409C-BE0B-7DC7F832D7E5}</author>
+    <author>tc={D9448BAA-F5B0-4321-90C2-A9D51981A62E}</author>
+    <author>tc={7AE7CF57-1275-4D06-A200-1594B54FC832}</author>
   </authors>
   <commentList>
     <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00C10032-00C3-40CD-A151-0096006000FD}">
@@ -670,12 +673,39 @@
 From 6.8 mW to 9.9 mW</t>
       </text>
     </comment>
+    <comment ref="R98" authorId="62" shapeId="0" xr:uid="{2C8311BA-9217-409C-BE0B-7DC7F832D7E5}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Only total power reported
+</t>
+      </text>
+    </comment>
+    <comment ref="L99" authorId="63" shapeId="0" xr:uid="{D9448BAA-F5B0-4321-90C2-A9D51981A62E}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Estimated
+</t>
+      </text>
+    </comment>
+    <comment ref="R101" authorId="64" shapeId="0" xr:uid="{7AE7CF57-1275-4D06-A200-1594B54FC832}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Only total power reported
+</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="383">
   <si>
     <t>DOI</t>
   </si>
@@ -1798,6 +1828,51 @@
   </si>
   <si>
     <t>Implementation of a dual-core Class-C topology utilizing switchable transformers, 7-bit switched capacitor arrays, and a noise-filtering technique (degeneration inductor) to block second-harmonic current.</t>
+  </si>
+  <si>
+    <t>10.1109/LMWC.2018.2890087</t>
+  </si>
+  <si>
+    <t>An Ultralow Phase Noise Eight-Core Fundamental 62-to-67-GHz VCO in 65-nm CMOS</t>
+  </si>
+  <si>
+    <t>Coupling eight VCOs using a scalable layout methodology (connecting coupled-VCO cells via extended lines) to achieve a 9-dB phase noise improvement.</t>
+  </si>
+  <si>
+    <t>10.23919/EUMIC61603.2024.10732408</t>
+  </si>
+  <si>
+    <t>Use of a dual-core topology with inductive coupling through a 2:1 side-coupled transformer (T1) to filter noise, provide bias, and extract the second harmonic non-invasively for push-push operation.</t>
+  </si>
+  <si>
+    <t>10.23919/RFIC.2018.8428984</t>
+  </si>
+  <si>
+    <t>A 31.8-40.8GHz Continuously Wide-Tuning VCO Based on Class-B Oscillator using Single Varactor and Inductor</t>
+  </si>
+  <si>
+    <t>Adoption of a push-pull complementary class-B oscillator (cascoded NMOS/PMOS Colpitts) to isolate the LC-tank and provide higher negative resistance, extending the tuning range without using switched capacitor banks or transformers.</t>
+  </si>
+  <si>
+    <t>Radio Frequency Integrated Circuits Symposium (RFIC)</t>
+  </si>
+  <si>
+    <t>10.23919/GeMiC64734.2025.10979128</t>
+  </si>
+  <si>
+    <t>A Low Phase-Noise Ka-band GHz VCO in 22 nm FDSOI CMOS for 6G Applications</t>
+  </si>
+  <si>
+    <t>Design of a low-phase-noise Ka-band VCO using a classic NMOS cross-coupled LC oscillator with H2 extraction from the common-mode tail node via a transformer to save power in the LO distribution network.</t>
+  </si>
+  <si>
+    <t>10.23919/EuMIC54514.2022.9923812</t>
+  </si>
+  <si>
+    <t>A 30-GHz CMOS LC VCO with Optimal Tail Filter Considering Tail FET’s Output Resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use of an Rt*Ct low-pass filter at the tail FET's gate node to boost output resistance (rds) and suppress noise, combined with an LC tail filter and inter-stage LC buffer matching to improve phase noise. </t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1883,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1847,6 +1922,18 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1878,7 +1965,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1909,6 +1996,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2492,6 +2582,18 @@
     <text>Only total power reported
 From 6.8 mW to 9.9 mW</text>
   </threadedComment>
+  <threadedComment ref="R98" personId="{6E22B2BB-0705-F6EB-A4FF-EDAEBE9386D7}" id="{2C8311BA-9217-409C-BE0B-7DC7F832D7E5}">
+    <text xml:space="preserve">Only total power reported
+</text>
+  </threadedComment>
+  <threadedComment ref="L99" personId="{6E22B2BB-0705-F6EB-A4FF-EDAEBE9386D7}" id="{D9448BAA-F5B0-4321-90C2-A9D51981A62E}">
+    <text xml:space="preserve">Estimated
+</text>
+  </threadedComment>
+  <threadedComment ref="R101" personId="{6E22B2BB-0705-F6EB-A4FF-EDAEBE9386D7}" id="{7AE7CF57-1275-4D06-A200-1594B54FC832}">
+    <text xml:space="preserve">Only total power reported
+</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2500,9 +2602,9 @@
   <dimension ref="A1:Z1043"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L4" sqref="L4"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="P103" sqref="P103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2689,7 +2791,7 @@
         <v>-182.46798907750107</v>
       </c>
       <c r="Z2" s="8">
-        <f>W2-20*LOG10(O2*1000000000/(V2*1000000))+10*LOG10(R2)-20*LOG(Q2/10)</f>
+        <f t="shared" ref="Z2:Z16" si="3">W2-20*LOG10(O2*1000000000/(V2*1000000))+10*LOG10(R2)-20*LOG(Q2/10)</f>
         <v>-177.73654894875983</v>
       </c>
     </row>
@@ -2773,7 +2875,7 @@
         <v>-172.28452800205508</v>
       </c>
       <c r="Z3" s="8">
-        <f>W3-20*LOG10(O3*1000000000/(V3*1000000))+10*LOG10(R3)-20*LOG(Q3/10)</f>
+        <f t="shared" si="3"/>
         <v>-156.36692765517358</v>
       </c>
     </row>
@@ -2858,7 +2960,7 @@
         <v>-179.48825754386067</v>
       </c>
       <c r="Z4" s="8">
-        <f>W4-20*LOG10(O4*1000000000/(V4*1000000))+10*LOG10(R4)-20*LOG(Q4/10)</f>
+        <f t="shared" si="3"/>
         <v>-175.81308354369634</v>
       </c>
     </row>
@@ -2942,7 +3044,7 @@
         <v>-175.47825568332235</v>
       </c>
       <c r="Z5" s="8">
-        <f>W5-20*LOG10(O5*1000000000/(V5*1000000))+10*LOG10(R5)-20*LOG(Q5/10)</f>
+        <f t="shared" si="3"/>
         <v>-167.07392761565856</v>
       </c>
     </row>
@@ -3027,7 +3129,7 @@
         <v>-172.66819770390885</v>
       </c>
       <c r="Z6" s="8">
-        <f>W6-20*LOG10(O6*1000000000/(V6*1000000))+10*LOG10(R6)-20*LOG(Q6/10)</f>
+        <f t="shared" si="3"/>
         <v>-165.92335433754033</v>
       </c>
     </row>
@@ -3111,7 +3213,7 @@
         <v>-179.27991572814545</v>
       </c>
       <c r="Z7" s="8">
-        <f>W7-20*LOG10(O7*1000000000/(V7*1000000))+10*LOG10(R7)-20*LOG(Q7/10)</f>
+        <f t="shared" si="3"/>
         <v>-150.16127661515097</v>
       </c>
     </row>
@@ -3195,7 +3297,7 @@
         <v>-190.53586023660267</v>
       </c>
       <c r="Z8" s="8">
-        <f>W8-20*LOG10(O8*1000000000/(V8*1000000))+10*LOG10(R8)-20*LOG(Q8/10)</f>
+        <f t="shared" si="3"/>
         <v>-184.68726375856141</v>
       </c>
     </row>
@@ -3279,7 +3381,7 @@
         <v>-190.62850055101376</v>
       </c>
       <c r="Z9" s="8">
-        <f>W9-20*LOG10(O9*1000000000/(V9*1000000))+10*LOG10(R9)-20*LOG(Q9/10)</f>
+        <f t="shared" si="3"/>
         <v>-192.21212547196626</v>
       </c>
     </row>
@@ -3364,7 +3466,7 @@
         <v>-184.12657491473067</v>
       </c>
       <c r="Z10" s="8">
-        <f>W10-20*LOG10(O10*1000000000/(V10*1000000))+10*LOG10(R10)-20*LOG(Q10/10)</f>
+        <f t="shared" si="3"/>
         <v>-181.62780018256467</v>
       </c>
     </row>
@@ -3448,7 +3550,7 @@
         <v>-184.14602621771584</v>
       </c>
       <c r="Z11" s="8">
-        <f>W11-20*LOG10(O11*1000000000/(V11*1000000))+10*LOG10(R11)-20*LOG(Q11/10)</f>
+        <f t="shared" si="3"/>
         <v>-163.23087640650235</v>
       </c>
     </row>
@@ -3531,7 +3633,7 @@
         <v>-187.92393759822966</v>
       </c>
       <c r="Z12" s="8">
-        <f>W12-20*LOG10(O12*1000000000/(V12*1000000))+10*LOG10(R12)-20*LOG(Q12/10)</f>
+        <f t="shared" si="3"/>
         <v>-189.86213785839078</v>
       </c>
     </row>
@@ -3615,7 +3717,7 @@
         <v>-174.11645041927852</v>
       </c>
       <c r="Z13" s="8">
-        <f>W13-20*LOG10(O13*1000000000/(V13*1000000))+10*LOG10(R13)-20*LOG(Q13/10)</f>
+        <f t="shared" si="3"/>
         <v>-186.30833860378291</v>
       </c>
     </row>
@@ -3699,7 +3801,7 @@
         <v>-189.62416620350703</v>
       </c>
       <c r="Z14" s="8">
-        <f>W14-20*LOG10(O14*1000000000/(V14*1000000))+10*LOG10(R14)-20*LOG(Q14/10)</f>
+        <f t="shared" si="3"/>
         <v>-195.24483354846157</v>
       </c>
     </row>
@@ -3765,7 +3867,7 @@
         <v>-1.85</v>
       </c>
       <c r="U15" s="7">
-        <f t="shared" ref="U15:U24" si="3">10^(T15/10)/S15</f>
+        <f t="shared" ref="U15:U24" si="4">10^(T15/10)/S15</f>
         <v>6.1040238565184333E-2</v>
       </c>
       <c r="V15" s="6">
@@ -3783,7 +3885,7 @@
         <v>-190.27414759750405</v>
       </c>
       <c r="Z15" s="8">
-        <f>W15-20*LOG10(O15*1000000000/(V15*1000000))+10*LOG10(R15)-20*LOG(Q15/10)</f>
+        <f t="shared" si="3"/>
         <v>-202.24339160698707</v>
       </c>
     </row>
@@ -3851,7 +3953,7 @@
         <v>-1.5</v>
       </c>
       <c r="U16" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.9795697995965401E-3</v>
       </c>
       <c r="V16" s="6">
@@ -3869,7 +3971,7 @@
         <v>-180.41682140150627</v>
       </c>
       <c r="Z16" s="8">
-        <f>W16-20*LOG10(O16*1000000000/(V16*1000000))+10*LOG10(R16)-20*LOG(Q16/10)</f>
+        <f t="shared" si="3"/>
         <v>-182.69568844764299</v>
       </c>
     </row>
@@ -3935,7 +4037,7 @@
         <v>-10</v>
       </c>
       <c r="U17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2727272727272731E-3</v>
       </c>
       <c r="V17" s="6">
@@ -4017,7 +4119,7 @@
         <v>-9.3000000000000007</v>
       </c>
       <c r="U18" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.9744241897203268E-2</v>
       </c>
       <c r="V18" s="6">
@@ -4101,7 +4203,7 @@
         <v>-10</v>
       </c>
       <c r="U19" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2727272727272731E-3</v>
       </c>
       <c r="V19" s="6">
@@ -4184,7 +4286,7 @@
         <v>32</v>
       </c>
       <c r="U20" s="7" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="V20" s="6">
@@ -4198,11 +4300,11 @@
         <v>-119.8</v>
       </c>
       <c r="Y20" s="8">
-        <f t="shared" ref="Y20:Y51" si="4">W20-20*LOG10(O20*1000000000/(V20*1000000))+10*LOG10(R20)</f>
+        <f t="shared" ref="Y20:Y51" si="5">W20-20*LOG10(O20*1000000000/(V20*1000000))+10*LOG10(R20)</f>
         <v>-184.81048723519586</v>
       </c>
       <c r="Z20" s="8">
-        <f t="shared" ref="Z20:Z51" si="5">W20-20*LOG10(O20*1000000000/(V20*1000000))+10*LOG10(R20)-20*LOG(Q20/10)</f>
+        <f t="shared" ref="Z20:Z51" si="6">W20-20*LOG10(O20*1000000000/(V20*1000000))+10*LOG10(R20)-20*LOG(Q20/10)</f>
         <v>-188.67297920228509</v>
       </c>
     </row>
@@ -4269,7 +4371,7 @@
         <v>-10</v>
       </c>
       <c r="U21" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.0816326530612249E-3</v>
       </c>
       <c r="V21" s="6">
@@ -4283,11 +4385,11 @@
         <v>-122</v>
       </c>
       <c r="Y21" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-181.03114787364638</v>
       </c>
       <c r="Z21" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-175.67902307010576</v>
       </c>
     </row>
@@ -4354,7 +4456,7 @@
         <v>1.7</v>
       </c>
       <c r="U22" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.8607225877880497E-2</v>
       </c>
       <c r="V22" s="6">
@@ -4368,11 +4470,11 @@
         <v>-111.3</v>
       </c>
       <c r="Y22" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-170.84386101598645</v>
       </c>
       <c r="Z22" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-177.3295101219403</v>
       </c>
     </row>
@@ -4439,7 +4541,7 @@
         <v>-4</v>
       </c>
       <c r="U23" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.903011476014679E-2</v>
       </c>
       <c r="V23" s="6">
@@ -4453,11 +4555,11 @@
         <v>-99.6</v>
       </c>
       <c r="Y23" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-178.9983235639059</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-169.4992197046428</v>
       </c>
     </row>
@@ -4523,7 +4625,7 @@
         <v>-3.5</v>
       </c>
       <c r="U24" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3535866428817066E-2</v>
       </c>
       <c r="V24" s="6">
@@ -4537,11 +4639,11 @@
         <v>-91.8</v>
       </c>
       <c r="Y24" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-165.1515896772913</v>
       </c>
       <c r="Z24" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-165.2894638362493</v>
       </c>
     </row>
@@ -4620,11 +4722,11 @@
         <v>-105</v>
       </c>
       <c r="Y25" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-181.7137800269083</v>
       </c>
       <c r="Z25" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-176.03384689960427</v>
       </c>
     </row>
@@ -4704,11 +4806,11 @@
         <v>-109.17</v>
       </c>
       <c r="Y26" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-171.43006147269648</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-174.41444372580409</v>
       </c>
     </row>
@@ -4788,11 +4890,11 @@
         <v>-115.9</v>
       </c>
       <c r="Y27" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-181.81923829585429</v>
       </c>
       <c r="Z27" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-182.15990508182989</v>
       </c>
     </row>
@@ -4872,11 +4974,11 @@
         <v>-124</v>
       </c>
       <c r="Y28" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-184.38793132739045</v>
       </c>
       <c r="Z28" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-184.89404863268587</v>
       </c>
     </row>
@@ -4956,11 +5058,11 @@
         <v>-103.6</v>
       </c>
       <c r="Y29" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-169.12923608346489</v>
       </c>
       <c r="Z29" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-171.59319758410487</v>
       </c>
     </row>
@@ -5040,11 +5142,11 @@
         <v>-124.7</v>
       </c>
       <c r="Y30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-185.92346966255079</v>
       </c>
       <c r="Z30" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-188.96923655021192</v>
       </c>
     </row>
@@ -5127,11 +5229,11 @@
         <v>-127.5</v>
       </c>
       <c r="Y31" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-184.77502343778519</v>
       </c>
       <c r="Z31" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-194.65811531815405</v>
       </c>
     </row>
@@ -5210,11 +5312,11 @@
         <v>-127.2</v>
       </c>
       <c r="Y32" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-187.60389194783613</v>
       </c>
       <c r="Z32" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-189.1294170559205</v>
       </c>
     </row>
@@ -5281,7 +5383,7 @@
         <v>2.8</v>
       </c>
       <c r="U33" s="7">
-        <f t="shared" ref="U33:U39" si="6">10^(T33/10)/S33</f>
+        <f t="shared" ref="U33:U39" si="7">10^(T33/10)/S33</f>
         <v>2.802148114651834E-2</v>
       </c>
       <c r="V33" s="6">
@@ -5295,11 +5397,11 @@
         <v>-96</v>
       </c>
       <c r="Y33" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-167.24624078481449</v>
       </c>
       <c r="Z33" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-155.87351606799425</v>
       </c>
     </row>
@@ -5366,7 +5468,7 @@
         <v>4.3</v>
       </c>
       <c r="U34" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.4858913398781931E-2</v>
       </c>
       <c r="V34" s="6">
@@ -5376,15 +5478,15 @@
         <v>-112</v>
       </c>
       <c r="X34" s="6">
-        <f t="shared" ref="X34:X65" si="7">W34+20*LOG10(V34/10)</f>
+        <f t="shared" ref="X34:X65" si="8">W34+20*LOG10(V34/10)</f>
         <v>-112</v>
       </c>
       <c r="Y34" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-173.35145908026763</v>
       </c>
       <c r="Z34" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-174.64061886480599</v>
       </c>
     </row>
@@ -5450,7 +5552,7 @@
         <v>-9.3000000000000007</v>
       </c>
       <c r="U35" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9744241897203268E-2</v>
       </c>
       <c r="V35" s="6">
@@ -5460,15 +5562,15 @@
         <v>-119.16</v>
       </c>
       <c r="X35" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-119.16</v>
       </c>
       <c r="Y35" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-191.14657086954421</v>
       </c>
       <c r="Z35" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-188.29322079816959</v>
       </c>
     </row>
@@ -5534,7 +5636,7 @@
         <v>-4</v>
       </c>
       <c r="U36" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8764086714069834E-3</v>
       </c>
       <c r="V36" s="6">
@@ -5544,15 +5646,15 @@
         <v>-125.4</v>
       </c>
       <c r="X36" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-125.4</v>
       </c>
       <c r="Y36" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-183.23683738983604</v>
       </c>
       <c r="Z36" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-180.38348731846142</v>
       </c>
     </row>
@@ -5618,7 +5720,7 @@
         <v>-10.1</v>
       </c>
       <c r="U37" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1023403839867004E-3</v>
       </c>
       <c r="V37" s="6">
@@ -5628,15 +5730,15 @@
         <v>-112.1</v>
       </c>
       <c r="X37" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-112.1</v>
       </c>
       <c r="Y37" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-177.3638359089245</v>
       </c>
       <c r="Z37" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-167.46683547532263</v>
       </c>
     </row>
@@ -5703,7 +5805,7 @@
         <v>3</v>
       </c>
       <c r="U38" s="7" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="V38" s="6">
@@ -5713,15 +5815,15 @@
         <v>-121.7</v>
       </c>
       <c r="X38" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-121.7</v>
       </c>
       <c r="Y38" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-185.32808342518302</v>
       </c>
       <c r="Z38" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-187.87017939247917</v>
       </c>
     </row>
@@ -5788,7 +5890,7 @@
         <v>5.46</v>
       </c>
       <c r="U39" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.0518815997743667E-2</v>
       </c>
       <c r="V39" s="6">
@@ -5798,15 +5900,15 @@
         <v>-117.6</v>
       </c>
       <c r="X39" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-117.6</v>
       </c>
       <c r="Y39" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-174.55912326978174</v>
       </c>
       <c r="Z39" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-178.8028753578609</v>
       </c>
     </row>
@@ -5881,15 +5983,15 @@
         <v>-122.05</v>
       </c>
       <c r="X40" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-122.05</v>
       </c>
       <c r="Y40" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-188.45029470562784</v>
       </c>
       <c r="Z40" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-170.31872840887254</v>
       </c>
     </row>
@@ -5966,15 +6068,15 @@
         <v>-98</v>
       </c>
       <c r="X41" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-118</v>
       </c>
       <c r="Y41" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-186.45189268768274</v>
       </c>
       <c r="Z41" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-182.93006750656912</v>
       </c>
     </row>
@@ -6050,15 +6152,15 @@
         <v>189</v>
       </c>
       <c r="X42" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-96.51</v>
       </c>
       <c r="Y42" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-161.14953939975956</v>
       </c>
       <c r="Z42" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-159.93992445213192</v>
       </c>
     </row>
@@ -6134,15 +6236,15 @@
         <v>-109.22</v>
       </c>
       <c r="X43" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-109.22</v>
       </c>
       <c r="Y43" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-174.26103221782415</v>
       </c>
       <c r="Z43" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-161.26599258450742</v>
       </c>
     </row>
@@ -6220,15 +6322,15 @@
         <v>-115.1</v>
       </c>
       <c r="X44" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-115.1</v>
       </c>
       <c r="Y44" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-181.07382040543479</v>
       </c>
       <c r="Z44" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-171.31148762501226</v>
       </c>
     </row>
@@ -6304,15 +6406,15 @@
         <v>-89</v>
       </c>
       <c r="X45" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-109</v>
       </c>
       <c r="Y45" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-174.36176445845595</v>
       </c>
       <c r="Z45" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-170.0255382799611</v>
       </c>
     </row>
@@ -6387,15 +6489,15 @@
         <v>-104.7</v>
       </c>
       <c r="X46" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-124.7</v>
       </c>
       <c r="Y46" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-186.60992443651148</v>
       </c>
       <c r="Z46" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-189.65569132417261</v>
       </c>
     </row>
@@ -6472,15 +6574,15 @@
         <v>-99</v>
       </c>
       <c r="X47" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-119</v>
       </c>
       <c r="Y47" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-175.61064778433783</v>
       </c>
       <c r="Z47" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-181.84572500545292</v>
       </c>
     </row>
@@ -6556,15 +6658,15 @@
         <v>-98.03</v>
       </c>
       <c r="X48" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-98.03</v>
       </c>
       <c r="Y48" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-171.70983678803088</v>
       </c>
       <c r="Z48" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-163.75103661459013</v>
       </c>
     </row>
@@ -6640,15 +6742,15 @@
         <v>-105.8</v>
       </c>
       <c r="X49" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-105.8</v>
       </c>
       <c r="Y49" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-170.09636353317259</v>
       </c>
       <c r="Z49" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-168.53009304284464</v>
       </c>
     </row>
@@ -6726,15 +6828,15 @@
         <v>-107.5</v>
       </c>
       <c r="X50" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-107.5</v>
       </c>
       <c r="Y50" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-178.79486364359022</v>
       </c>
       <c r="Z50" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-168.89786320998834</v>
       </c>
     </row>
@@ -6811,15 +6913,15 @@
         <v>-115</v>
       </c>
       <c r="X51" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-115</v>
       </c>
       <c r="Y51" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-185.18996489706842</v>
       </c>
       <c r="Z51" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-178.79667516535969</v>
       </c>
     </row>
@@ -6896,15 +6998,15 @@
         <v>-114.63</v>
       </c>
       <c r="X52" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-114.63</v>
       </c>
       <c r="Y52" s="8">
-        <f t="shared" ref="Y52:Y77" si="8">W52-20*LOG10(O52*1000000000/(V52*1000000))+10*LOG10(R52)</f>
+        <f t="shared" ref="Y52:Y77" si="9">W52-20*LOG10(O52*1000000000/(V52*1000000))+10*LOG10(R52)</f>
         <v>-182.21552370284391</v>
       </c>
       <c r="Z52" s="8">
-        <f t="shared" ref="Z52:Z77" si="9">W52-20*LOG10(O52*1000000000/(V52*1000000))+10*LOG10(R52)-20*LOG(Q52/10)</f>
+        <f t="shared" ref="Z52:Z77" si="10">W52-20*LOG10(O52*1000000000/(V52*1000000))+10*LOG10(R52)-20*LOG(Q52/10)</f>
         <v>-184.74151095662401</v>
       </c>
     </row>
@@ -6980,15 +7082,15 @@
         <v>-114.63</v>
       </c>
       <c r="X53" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-114.63</v>
       </c>
       <c r="Y53" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-181.83896499497399</v>
       </c>
       <c r="Z53" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-188.99766193498306</v>
       </c>
     </row>
@@ -7064,15 +7166,15 @@
         <v>-101.3</v>
       </c>
       <c r="X54" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-121.3</v>
       </c>
       <c r="Y54" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-182.58409211243236</v>
       </c>
       <c r="Z54" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-165.72359148460455</v>
       </c>
     </row>
@@ -7138,7 +7240,7 @@
         <v>-4</v>
       </c>
       <c r="U55" s="7">
-        <f t="shared" ref="U55:U67" si="10">10^(T55/10)/S55</f>
+        <f t="shared" ref="U55:U67" si="11">10^(T55/10)/S55</f>
         <v>3.1848573644279773E-2</v>
       </c>
       <c r="V55" s="6">
@@ -7148,15 +7250,15 @@
         <v>-95</v>
       </c>
       <c r="X55" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-95</v>
       </c>
       <c r="Y55" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-173.85813374660489</v>
       </c>
       <c r="Z55" s="8" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -7224,7 +7326,7 @@
         <v>0.79</v>
       </c>
       <c r="U56" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.2748430217650785E-2</v>
       </c>
       <c r="V56" s="6">
@@ -7234,15 +7336,15 @@
         <v>-113.9</v>
       </c>
       <c r="X56" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-113.9</v>
       </c>
       <c r="Y56" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-186.86700298778931</v>
       </c>
       <c r="Z56" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-170.94940264090781</v>
       </c>
     </row>
@@ -7310,7 +7412,7 @@
         <v>1</v>
       </c>
       <c r="U57" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.14810887197578437</v>
       </c>
       <c r="V57" s="6">
@@ -7320,15 +7422,15 @@
         <v>-111.6</v>
       </c>
       <c r="X57" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-111.6</v>
       </c>
       <c r="Y57" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-180.97049331715323</v>
       </c>
       <c r="Z57" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-179.35205516467471</v>
       </c>
     </row>
@@ -7395,7 +7497,7 @@
         <v>-6.6</v>
       </c>
       <c r="U58" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.6358573782524732E-2</v>
       </c>
       <c r="V58" s="6">
@@ -7405,15 +7507,15 @@
         <v>-91.2</v>
       </c>
       <c r="X58" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-111.2</v>
       </c>
       <c r="Y58" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-182.06457245602988</v>
       </c>
       <c r="Z58" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-181.80000714135477</v>
       </c>
     </row>
@@ -7479,7 +7581,7 @@
         <v>-21.1</v>
       </c>
       <c r="U59" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0213777850377512E-4</v>
       </c>
       <c r="V59" s="6">
@@ -7489,15 +7591,15 @@
         <v>-94.4</v>
       </c>
       <c r="X59" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-114.4</v>
       </c>
       <c r="Y59" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-177.84786213384962</v>
       </c>
       <c r="Z59" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-181.93026178696812</v>
       </c>
     </row>
@@ -7563,7 +7665,7 @@
         <v>-6.4</v>
       </c>
       <c r="U60" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.6132870794139248E-2</v>
       </c>
       <c r="V60" s="6">
@@ -7573,15 +7675,15 @@
         <v>-111.9</v>
       </c>
       <c r="X60" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-111.9</v>
       </c>
       <c r="Y60" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-178.78333689490233</v>
       </c>
       <c r="Z60" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-183.88878699696846</v>
       </c>
     </row>
@@ -7647,7 +7749,7 @@
         <v>-17.8</v>
       </c>
       <c r="U61" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.6112494246966593E-3</v>
       </c>
       <c r="V61" s="6">
@@ -7657,15 +7759,15 @@
         <v>-122.1</v>
       </c>
       <c r="X61" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-122.1</v>
       </c>
       <c r="Y61" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-186.88183660961923</v>
       </c>
       <c r="Z61" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-192.945757758029</v>
       </c>
     </row>
@@ -7732,7 +7834,7 @@
         <v>3</v>
       </c>
       <c r="U62" s="7" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="V62" s="6">
@@ -7742,15 +7844,15 @@
         <v>-94</v>
       </c>
       <c r="X62" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-114</v>
       </c>
       <c r="Y62" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-182.71856123516488</v>
       </c>
       <c r="Z62" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-177.25310541569633</v>
       </c>
     </row>
@@ -7816,7 +7918,7 @@
         <v>-1</v>
       </c>
       <c r="U63" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.9072020410807081E-2</v>
       </c>
       <c r="V63" s="6">
@@ -7826,15 +7928,15 @@
         <v>-114.9</v>
       </c>
       <c r="X63" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-114.9</v>
       </c>
       <c r="Y63" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-190.86061366523865</v>
       </c>
       <c r="Z63" s="8" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -7900,7 +8002,7 @@
         <v>-6.93</v>
       </c>
       <c r="U64" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.0347699985752443E-2</v>
       </c>
       <c r="V64" s="6">
@@ -7910,15 +8012,15 @@
         <v>-114.5</v>
       </c>
       <c r="X64" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-114.5</v>
       </c>
       <c r="Y64" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-195.80419929487633</v>
       </c>
       <c r="Z64" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-183.03875601522819</v>
       </c>
     </row>
@@ -7985,7 +8087,7 @@
         <v>4.5</v>
       </c>
       <c r="U65" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.1269194157922917E-2</v>
       </c>
       <c r="V65" s="1">
@@ -7995,15 +8097,15 @@
         <v>-87</v>
       </c>
       <c r="X65" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-107</v>
       </c>
       <c r="Y65" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-169.55324952960615</v>
       </c>
       <c r="Z65" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-143.53264961632652</v>
       </c>
     </row>
@@ -8070,7 +8172,7 @@
         <v>7.5</v>
       </c>
       <c r="U66" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.1939108017897756</v>
       </c>
       <c r="V66" s="6">
@@ -8080,15 +8182,15 @@
         <v>-106.9</v>
       </c>
       <c r="X66" s="6">
-        <f t="shared" ref="X66:X97" si="11">W66+20*LOG10(V66/10)</f>
+        <f t="shared" ref="X66:X77" si="12">W66+20*LOG10(V66/10)</f>
         <v>-126.9</v>
       </c>
       <c r="Y66" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-191.16567346401382</v>
       </c>
       <c r="Z66" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-172.27602002101045</v>
       </c>
     </row>
@@ -8156,7 +8258,7 @@
         <v>-25</v>
       </c>
       <c r="U67" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.5175395145262518E-4</v>
       </c>
       <c r="V67" s="6">
@@ -8166,15 +8268,15 @@
         <v>-105.5</v>
       </c>
       <c r="X67" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-105.5</v>
       </c>
       <c r="Y67" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-177.09808935333442</v>
       </c>
       <c r="Z67" s="8" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -8249,15 +8351,15 @@
         <v>-94</v>
       </c>
       <c r="X68" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-114</v>
       </c>
       <c r="Y68" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-186.23978188319177</v>
       </c>
       <c r="Z68" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-184.07053103664305</v>
       </c>
     </row>
@@ -8323,7 +8425,7 @@
         <v>-15.6</v>
       </c>
       <c r="U69" s="7">
-        <f t="shared" ref="U69:U75" si="12">10^(T69/10)/S69</f>
+        <f t="shared" ref="U69:U75" si="13">10^(T69/10)/S69</f>
         <v>4.0503363284384776E-4</v>
       </c>
       <c r="V69" s="6">
@@ -8333,15 +8435,15 @@
         <v>-93</v>
       </c>
       <c r="X69" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-113</v>
       </c>
       <c r="Y69" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-174.97538989839228</v>
       </c>
       <c r="Z69" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-184.51781499278553</v>
       </c>
     </row>
@@ -8407,7 +8509,7 @@
         <v>-23</v>
       </c>
       <c r="U70" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.1364789878169435E-4</v>
       </c>
       <c r="V70" s="6">
@@ -8417,15 +8519,15 @@
         <v>-87</v>
       </c>
       <c r="X70" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-107</v>
       </c>
       <c r="Y70" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-172.14909815609062</v>
       </c>
       <c r="Z70" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-176.23149780920912</v>
       </c>
     </row>
@@ -8492,7 +8594,7 @@
         <v>6.5</v>
       </c>
       <c r="U71" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.15193319460917115</v>
       </c>
       <c r="V71" s="6">
@@ -8502,15 +8604,15 @@
         <v>-98.6</v>
       </c>
       <c r="X71" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-118.6</v>
       </c>
       <c r="Y71" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-189.7172189231288</v>
       </c>
       <c r="Z71" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-170.54507262629329</v>
       </c>
     </row>
@@ -8576,7 +8678,7 @@
         <v>4.8</v>
       </c>
       <c r="U72" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.11705239226364404</v>
       </c>
       <c r="V72" s="6">
@@ -8586,15 +8688,15 @@
         <v>-101.7</v>
       </c>
       <c r="X72" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-121.7</v>
       </c>
       <c r="Y72" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-192.47429317176938</v>
       </c>
       <c r="Z72" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-163.10387151261449</v>
       </c>
     </row>
@@ -8662,7 +8764,7 @@
         <v>-2</v>
       </c>
       <c r="U73" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.2371712636866533E-2</v>
       </c>
       <c r="V73" s="6">
@@ -8672,15 +8774,15 @@
         <v>-96.5</v>
       </c>
       <c r="X73" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-116.5</v>
       </c>
       <c r="Y73" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-181.89479785787529</v>
       </c>
       <c r="Z73" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-185.1221579025748</v>
       </c>
     </row>
@@ -8747,7 +8849,7 @@
         <v>-22.2</v>
       </c>
       <c r="U74" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9.2701474780670419E-5</v>
       </c>
       <c r="V74" s="6">
@@ -8757,15 +8859,15 @@
         <v>-94</v>
       </c>
       <c r="X74" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-114</v>
       </c>
       <c r="Y74" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-172.26174514440882</v>
       </c>
       <c r="Z74" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-183.38779515975457</v>
       </c>
     </row>
@@ -8832,7 +8934,7 @@
         <v>-20</v>
       </c>
       <c r="U75" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.5151515151515152E-4</v>
       </c>
       <c r="V75" s="6">
@@ -8842,15 +8944,15 @@
         <v>-91.8</v>
       </c>
       <c r="X75" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-111.8</v>
       </c>
       <c r="Y75" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-171.31338745531588</v>
       </c>
       <c r="Z75" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-179.27218762875663</v>
       </c>
     </row>
@@ -8925,15 +9027,15 @@
         <v>-100.7</v>
       </c>
       <c r="X76" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-120.7</v>
       </c>
       <c r="Y76" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-177.99727099740903</v>
       </c>
       <c r="Z76" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-181.97041273649748</v>
       </c>
     </row>
@@ -9008,15 +9110,15 @@
         <v>-91</v>
       </c>
       <c r="X77" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-111</v>
       </c>
       <c r="Y77" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-175.17194807964776</v>
       </c>
       <c r="Z77" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-182.70348722077802</v>
       </c>
     </row>
@@ -9173,7 +9275,7 @@
         <v>-106.9</v>
       </c>
       <c r="X79" s="6">
-        <f t="shared" ref="X79:X97" si="13">W79+20*LOG10(V79/10)</f>
+        <f t="shared" ref="X79:X99" si="14">W79+20*LOG10(V79/10)</f>
         <v>-106.9</v>
       </c>
       <c r="Y79" s="8">
@@ -9256,7 +9358,7 @@
         <v>-108.3</v>
       </c>
       <c r="X80" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-108.3</v>
       </c>
       <c r="Y80" s="8">
@@ -9340,7 +9442,7 @@
         <v>-99</v>
       </c>
       <c r="X81" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-119</v>
       </c>
       <c r="Y81" s="8">
@@ -9423,7 +9525,7 @@
         <v>-105.5</v>
       </c>
       <c r="X82" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-105.5</v>
       </c>
       <c r="Y82" s="8">
@@ -9508,7 +9610,7 @@
         <v>-124.75</v>
       </c>
       <c r="X83" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-124.75</v>
       </c>
       <c r="Y83" s="8">
@@ -9591,7 +9693,7 @@
         <v>-140</v>
       </c>
       <c r="X84" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-140</v>
       </c>
       <c r="Y84" s="8">
@@ -9664,7 +9766,7 @@
         <v>-4.8</v>
       </c>
       <c r="U85" s="7">
-        <f t="shared" ref="U85:U94" si="14">10^(T85/10)/S85</f>
+        <f t="shared" ref="U85:U94" si="15">10^(T85/10)/S85</f>
         <v>1.7898979539599517E-2</v>
       </c>
       <c r="V85" s="6">
@@ -9674,15 +9776,15 @@
         <v>-110.9</v>
       </c>
       <c r="X85" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-110.9</v>
       </c>
       <c r="Y85" s="8">
-        <f t="shared" ref="Y85:Y94" si="15">W85-20*LOG10(O85*1000000000/(V85*1000000))+10*LOG10(R85)</f>
+        <f t="shared" ref="Y85:Y94" si="16">W85-20*LOG10(O85*1000000000/(V85*1000000))+10*LOG10(R85)</f>
         <v>-185.79624073493261</v>
       </c>
       <c r="Z85" s="8">
-        <f t="shared" ref="Z85:Z94" si="16">W85-20*LOG10(O85*1000000000/(V85*1000000))+10*LOG10(R85)-20*LOG(Q85/10)</f>
+        <f t="shared" ref="Z85:Z94" si="17">W85-20*LOG10(O85*1000000000/(V85*1000000))+10*LOG10(R85)-20*LOG(Q85/10)</f>
         <v>-187.73444099509373</v>
       </c>
     </row>
@@ -9751,7 +9853,7 @@
         <v>1.3</v>
       </c>
       <c r="U86" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.4980794122067662E-2</v>
       </c>
       <c r="V86" s="6">
@@ -9761,15 +9863,15 @@
         <v>-66</v>
       </c>
       <c r="X86" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-86</v>
       </c>
       <c r="Y86" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-155.24773139605435</v>
       </c>
       <c r="Z86" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-151.63861010689172</v>
       </c>
     </row>
@@ -9835,7 +9937,7 @@
         <v>-14.5</v>
       </c>
       <c r="U87" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.8559274787104242E-4</v>
       </c>
       <c r="V87" s="6">
@@ -9845,15 +9947,15 @@
         <v>-91.3</v>
       </c>
       <c r="X87" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-111.3</v>
       </c>
       <c r="Y87" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-180.33192790751897</v>
       </c>
       <c r="Z87" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-183.25448862108374</v>
       </c>
     </row>
@@ -9920,7 +10022,7 @@
         <v>9</v>
       </c>
       <c r="U88" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.0176381418506196E-2</v>
       </c>
       <c r="V88" s="6">
@@ -9930,15 +10032,15 @@
         <v>-116</v>
       </c>
       <c r="X88" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-116</v>
       </c>
       <c r="Y88" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-178.48808930429345</v>
       </c>
       <c r="Z88" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-176.32998135810305</v>
       </c>
     </row>
@@ -10005,7 +10107,7 @@
         <v>-8</v>
       </c>
       <c r="U89" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6683086236432771E-3</v>
       </c>
       <c r="V89" s="6">
@@ -10015,15 +10117,15 @@
         <v>-115.5</v>
       </c>
       <c r="X89" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-115.5</v>
       </c>
       <c r="Y89" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-178.95012399181104</v>
       </c>
       <c r="Z89" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-184.97072390509067</v>
       </c>
     </row>
@@ -10091,7 +10193,7 @@
         <v>-15</v>
       </c>
       <c r="U90" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.4963293098149508E-4</v>
       </c>
       <c r="V90" s="6">
@@ -10101,15 +10203,15 @@
         <v>-74.83</v>
       </c>
       <c r="X90" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-94.83</v>
       </c>
       <c r="Y90" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-158.00032751699177</v>
       </c>
       <c r="Z90" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-158.66075641064998</v>
       </c>
     </row>
@@ -10176,7 +10278,7 @@
         <v>-17</v>
       </c>
       <c r="U91" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.5962098519751034E-3</v>
       </c>
       <c r="V91" s="1">
@@ -10186,15 +10288,15 @@
         <v>-113.7</v>
       </c>
       <c r="X91" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-113.7</v>
       </c>
       <c r="Y91" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-182.83389943631755</v>
       </c>
       <c r="Z91" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-179.73586023660269</v>
       </c>
     </row>
@@ -10260,7 +10362,7 @@
         <v>-10</v>
       </c>
       <c r="U92" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.6511627906976744E-3</v>
       </c>
       <c r="V92" s="1">
@@ -10270,15 +10372,15 @@
         <v>-114.95</v>
       </c>
       <c r="X92" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-114.95</v>
       </c>
       <c r="Y92" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-177.58480827558787</v>
       </c>
       <c r="Z92" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-186.0168868129845</v>
       </c>
     </row>
@@ -10346,7 +10448,7 @@
         <v>-2.4500000000000002</v>
       </c>
       <c r="U93" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.6464931464348808E-2</v>
       </c>
       <c r="V93" s="6">
@@ -10356,15 +10458,15 @@
         <v>-91.53</v>
       </c>
       <c r="X93" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-111.53</v>
       </c>
       <c r="Y93" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-178.71296637694778</v>
       </c>
       <c r="Z93" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-177.23981530946088</v>
       </c>
     </row>
@@ -10432,7 +10534,7 @@
         <v>-28.8</v>
       </c>
       <c r="U94" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8.907140125381128E-5</v>
       </c>
       <c r="V94" s="6">
@@ -10442,15 +10544,15 @@
         <v>-93.5</v>
       </c>
       <c r="X94" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-113.5</v>
       </c>
       <c r="Y94" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-178.69303142461987</v>
       </c>
       <c r="Z94" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-183.40360036277085</v>
       </c>
     </row>
@@ -10526,7 +10628,7 @@
         <v>-124.75</v>
       </c>
       <c r="X95" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-124.75</v>
       </c>
       <c r="Y95" s="8">
@@ -10608,7 +10710,7 @@
         <v>-92.83</v>
       </c>
       <c r="X96" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-112.83</v>
       </c>
       <c r="Y96" s="8">
@@ -10691,7 +10793,7 @@
         <v>-116</v>
       </c>
       <c r="X97" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-116</v>
       </c>
       <c r="Y97" s="8">
@@ -10704,134 +10806,424 @@
       </c>
     </row>
     <row r="98" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
-      <c r="F98" s="6"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="6"/>
-      <c r="I98" s="6"/>
-      <c r="J98" s="6"/>
-      <c r="K98" s="6"/>
-      <c r="L98" s="6"/>
-      <c r="M98" s="6"/>
-      <c r="N98" s="6"/>
-      <c r="O98" s="6"/>
-      <c r="P98" s="6"/>
-      <c r="Q98" s="6"/>
-      <c r="R98" s="6"/>
-      <c r="S98" s="6"/>
-      <c r="T98" s="6"/>
-      <c r="U98" s="6"/>
-      <c r="V98" s="6"/>
-      <c r="W98" s="6"/>
-      <c r="X98" s="6"/>
+      <c r="A98" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E98" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L98" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="M98" s="6">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="N98" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O98" s="6">
+        <v>64.75</v>
+      </c>
+      <c r="P98" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q98" s="6">
+        <v>7.9</v>
+      </c>
+      <c r="R98" s="1">
+        <v>61.2</v>
+      </c>
+      <c r="S98" s="6">
+        <v>61.2</v>
+      </c>
+      <c r="T98" s="6">
+        <v>-11</v>
+      </c>
+      <c r="U98" s="7">
+        <f t="shared" ref="U98:U99" si="18">10^(T98/10)/S98</f>
+        <v>1.2979219521638578E-3</v>
+      </c>
+      <c r="V98" s="6">
+        <v>10</v>
+      </c>
+      <c r="W98" s="6">
+        <v>-122.6</v>
+      </c>
+      <c r="X98" s="6">
+        <f t="shared" si="14"/>
+        <v>-122.6</v>
+      </c>
+      <c r="Y98" s="8">
+        <f>W98-20*LOG10(O98*1000000000/(V98*1000000))+10*LOG10(R98)</f>
+        <v>-180.95728123361016</v>
+      </c>
+      <c r="Z98" s="8">
+        <f>W98-20*LOG10(O98*1000000000/(V98*1000000))+10*LOG10(R98)-20*LOG(Q98/10)</f>
+        <v>-178.90982305941898</v>
+      </c>
     </row>
     <row r="99" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
-      <c r="F99" s="6"/>
-      <c r="G99" s="6"/>
-      <c r="H99" s="6"/>
-      <c r="I99" s="6"/>
-      <c r="J99" s="6"/>
-      <c r="K99" s="6"/>
-      <c r="L99" s="6"/>
-      <c r="M99" s="6"/>
-      <c r="N99" s="6"/>
-      <c r="O99" s="6"/>
-      <c r="P99" s="6"/>
-      <c r="Q99" s="6"/>
-      <c r="R99" s="6"/>
-      <c r="S99" s="6"/>
-      <c r="T99" s="6"/>
-      <c r="U99" s="6"/>
-      <c r="V99" s="6"/>
-      <c r="W99" s="6"/>
-      <c r="X99" s="6"/>
+      <c r="A99" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E99" s="6">
+        <v>2024</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="H99" s="6">
+        <v>350</v>
+      </c>
+      <c r="I99" s="6">
+        <v>400</v>
+      </c>
+      <c r="J99" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K99" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L99" s="6">
+        <v>3.125E-2</v>
+      </c>
+      <c r="M99" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="N99" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O99" s="6">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="P99" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q99" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="R99" s="6">
+        <v>19.7</v>
+      </c>
+      <c r="S99" s="6">
+        <v>24.5</v>
+      </c>
+      <c r="T99" s="6">
+        <v>-10</v>
+      </c>
+      <c r="U99" s="7">
+        <f t="shared" si="18"/>
+        <v>4.0816326530612249E-3</v>
+      </c>
+      <c r="V99" s="6">
+        <v>10</v>
+      </c>
+      <c r="W99" s="6">
+        <v>-120.35</v>
+      </c>
+      <c r="X99" s="6">
+        <f t="shared" si="14"/>
+        <v>-120.35</v>
+      </c>
+      <c r="Y99" s="8">
+        <f>W99-20*LOG10(O99*1000000000/(V99*1000000))+10*LOG10(R99)</f>
+        <v>-179.59722592288847</v>
+      </c>
+      <c r="Z99" s="8">
+        <f>W99-20*LOG10(O99*1000000000/(V99*1000000))+10*LOG10(R99)-20*LOG(Q99/10)</f>
+        <v>-174.24510111934785</v>
+      </c>
     </row>
     <row r="100" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
-      <c r="F100" s="6"/>
-      <c r="G100" s="6"/>
-      <c r="H100" s="6"/>
-      <c r="I100" s="6"/>
-      <c r="J100" s="6"/>
-      <c r="K100" s="6"/>
-      <c r="L100" s="6"/>
-      <c r="M100" s="6"/>
-      <c r="N100" s="6"/>
-      <c r="O100" s="6"/>
-      <c r="P100" s="6"/>
-      <c r="Q100" s="6"/>
-      <c r="R100" s="6"/>
-      <c r="S100" s="6"/>
-      <c r="T100" s="6"/>
-      <c r="U100" s="6"/>
-      <c r="V100" s="6"/>
-      <c r="W100" s="6"/>
-      <c r="X100" s="6"/>
+      <c r="A100" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="E100" s="6">
+        <v>2018</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J100" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L100" s="6">
+        <v>2.7E-2</v>
+      </c>
+      <c r="M100" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N100" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O100" s="6">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="P100" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q100" s="6">
+        <v>24.8</v>
+      </c>
+      <c r="R100" s="6">
+        <v>20</v>
+      </c>
+      <c r="S100" s="6">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="T100" s="6">
+        <v>-12</v>
+      </c>
+      <c r="U100" s="7">
+        <f t="shared" ref="U100" si="19">10^(T100/10)/S100</f>
+        <v>1.5464640796083167E-3</v>
+      </c>
+      <c r="V100" s="6">
+        <v>10</v>
+      </c>
+      <c r="W100" s="6">
+        <v>-115</v>
+      </c>
+      <c r="X100" s="6">
+        <f t="shared" ref="X100" si="20">W100+20*LOG10(V100/10)</f>
+        <v>-115</v>
+      </c>
+      <c r="Y100" s="8">
+        <f>W100-20*LOG10(O100*1000000000/(V100*1000000))+10*LOG10(R100)</f>
+        <v>-173.18783254408243</v>
+      </c>
+      <c r="Z100" s="8">
+        <f>W100-20*LOG10(O100*1000000000/(V100*1000000))+10*LOG10(R100)-20*LOG(Q100/10)</f>
+        <v>-181.07686616060676</v>
+      </c>
     </row>
     <row r="101" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="6"/>
-      <c r="H101" s="6"/>
-      <c r="I101" s="6"/>
-      <c r="J101" s="6"/>
-      <c r="K101" s="6"/>
-      <c r="L101" s="6"/>
-      <c r="M101" s="6"/>
-      <c r="N101" s="6"/>
-      <c r="O101" s="6"/>
-      <c r="P101" s="6"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="6"/>
-      <c r="S101" s="6"/>
-      <c r="T101" s="6"/>
-      <c r="U101" s="6"/>
-      <c r="V101" s="6"/>
-      <c r="W101" s="6"/>
-      <c r="X101" s="6"/>
+      <c r="A101" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E101" s="6">
+        <v>2025</v>
+      </c>
+      <c r="F101" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G101" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="H101" s="6">
+        <v>350</v>
+      </c>
+      <c r="I101" s="6">
+        <v>400</v>
+      </c>
+      <c r="J101" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K101" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L101" s="6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M101" s="6">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="N101" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O101" s="6">
+        <v>28.8</v>
+      </c>
+      <c r="P101" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q101" s="6">
+        <v>8.66</v>
+      </c>
+      <c r="R101" s="1">
+        <v>31.2</v>
+      </c>
+      <c r="S101" s="6">
+        <v>31.2</v>
+      </c>
+      <c r="T101" s="6">
+        <v>-5.5</v>
+      </c>
+      <c r="U101" s="7">
+        <f t="shared" ref="U101:U102" si="21">10^(T101/10)/S101</f>
+        <v>9.0332786258476069E-3</v>
+      </c>
+      <c r="V101" s="6">
+        <v>10</v>
+      </c>
+      <c r="W101" s="6">
+        <v>-124.93</v>
+      </c>
+      <c r="X101" s="6">
+        <f t="shared" ref="X101:X102" si="22">W101+20*LOG10(V101/10)</f>
+        <v>-124.93</v>
+      </c>
+      <c r="Y101" s="8">
+        <f>W101-20*LOG10(O101*1000000000/(V101*1000000))+10*LOG10(R101)</f>
+        <v>-179.17630381500021</v>
+      </c>
+      <c r="Z101" s="8">
+        <f>W101-20*LOG10(O101*1000000000/(V101*1000000))+10*LOG10(R101)-20*LOG(Q101/10)</f>
+        <v>-177.92666165534715</v>
+      </c>
     </row>
     <row r="102" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="6"/>
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
-      <c r="F102" s="6"/>
-      <c r="G102" s="6"/>
-      <c r="H102" s="6"/>
-      <c r="I102" s="6"/>
-      <c r="J102" s="6"/>
-      <c r="K102" s="6"/>
-      <c r="L102" s="6"/>
-      <c r="M102" s="6"/>
-      <c r="N102" s="6"/>
-      <c r="O102" s="6"/>
-      <c r="P102" s="6"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="6"/>
-      <c r="S102" s="6"/>
-      <c r="T102" s="6"/>
-      <c r="U102" s="6"/>
-      <c r="V102" s="6"/>
-      <c r="W102" s="6"/>
-      <c r="X102" s="6"/>
+      <c r="A102" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E102" s="6">
+        <v>2022</v>
+      </c>
+      <c r="F102" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G102" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H102" s="6">
+        <v>170</v>
+      </c>
+      <c r="I102" s="6">
+        <v>200</v>
+      </c>
+      <c r="J102" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K102" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L102" s="6">
+        <v>0.254</v>
+      </c>
+      <c r="M102" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N102" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O102" s="6">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="P102" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q102" s="6">
+        <v>14.3</v>
+      </c>
+      <c r="R102" s="6">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="S102" s="6">
+        <v>35.880000000000003</v>
+      </c>
+      <c r="T102" s="6">
+        <v>-5.165</v>
+      </c>
+      <c r="U102" s="7">
+        <f t="shared" si="21"/>
+        <v>8.4849163601520092E-3</v>
+      </c>
+      <c r="V102" s="6">
+        <v>10</v>
+      </c>
+      <c r="W102" s="6">
+        <v>-129.6</v>
+      </c>
+      <c r="X102" s="6">
+        <f t="shared" si="22"/>
+        <v>-129.6</v>
+      </c>
+      <c r="Y102" s="8">
+        <f>W102-20*LOG10(O102*1000000000/(V102*1000000))+10*LOG10(R102)</f>
+        <v>-187.47825038777989</v>
+      </c>
+      <c r="Z102" s="8">
+        <f>W102-20*LOG10(O102*1000000000/(V102*1000000))+10*LOG10(R102)-20*LOG(Q102/10)</f>
+        <v>-190.58497113708114</v>
+      </c>
     </row>
     <row r="103" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="6"/>

</xml_diff>